<commit_message>
241203 T update and also fixed the final exam dates on the calendar
</commit_message>
<xml_diff>
--- a/Semester Planner-101-2024-fall.xlsx
+++ b/Semester Planner-101-2024-fall.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t xml:space="preserve">Input Start Info:</t>
   </si>
@@ -200,13 +200,16 @@
     <t xml:space="preserve">DEAD DAY</t>
   </si>
   <si>
+    <t xml:space="preserve">FINAL EXAM 8AM section 03</t>
+  </si>
+  <si>
     <t xml:space="preserve">FINAL EXAMS</t>
   </si>
   <si>
-    <t xml:space="preserve">FINAL EXAM 8AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FINAL EXAM 10:30AM</t>
+    <t xml:space="preserve">FINAL EXAM 1PM section 01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FINAL EXAM 8AM section 02</t>
   </si>
 </sst>
 </file>
@@ -393,35 +396,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -433,107 +436,107 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -676,15 +679,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A2:K103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K26" activeCellId="0" sqref="K26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G101" activeCellId="0" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -695,7 +804,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="48.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="3.41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.84"/>
@@ -2459,11 +2568,15 @@
         <f aca="false">IF(D97="",D96+IF(OR(WEEKDAY(D96)=2,WEEKDAY(D96)=4),2,3),"")</f>
         <v>45635</v>
       </c>
-      <c r="E98" s="16"/>
+      <c r="E98" s="16" t="s">
+        <v>49</v>
+      </c>
       <c r="F98" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="G98" s="16"/>
+        <v>50</v>
+      </c>
+      <c r="G98" s="16" t="s">
+        <v>51</v>
+      </c>
       <c r="H98" s="15" t="n">
         <f aca="false">H95+IF(WEEKDAY(H95)=3,2,5)</f>
         <v>45636</v>
@@ -2494,7 +2607,7 @@
         <v>45637</v>
       </c>
       <c r="E100" s="22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F100" s="16"/>
       <c r="G100" s="16"/>
@@ -2509,9 +2622,7 @@
       <c r="D101" s="21"/>
       <c r="E101" s="22"/>
       <c r="F101" s="22"/>
-      <c r="G101" s="22" t="s">
-        <v>51</v>
-      </c>
+      <c r="G101" s="22"/>
       <c r="H101" s="21" t="n">
         <f aca="false">H98+IF(WEEKDAY(H98)=3,2,5)</f>
         <v>45638</v>
@@ -2529,7 +2640,7 @@
       </c>
       <c r="E102" s="22"/>
       <c r="F102" s="16"/>
-      <c r="G102" s="16"/>
+      <c r="G102" s="22"/>
       <c r="H102" s="21"/>
       <c r="I102" s="20"/>
       <c r="J102" s="14"/>
@@ -2862,7 +2973,7 @@
       <formula>"not(isblank(address(row(),c)))"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B98 E98:G98 B102 E102:G102">
+  <conditionalFormatting sqref="B98 E98:F98 B102 E102:F102">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"not(isblank(address(row(),c)))"</formula>
     </cfRule>
@@ -2877,9 +2988,19 @@
       <formula>"not(isblank(address(row(),c)))"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G98">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"not(isblank(address(row(),c)))"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G102">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"not(isblank(address(row(),c)))"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>